<commit_message>
adding writing on excel
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/notthefinalproject/test.xlsx
+++ b/src/main/java/com/example/notthefinalproject/test.xlsx
@@ -443,4 +443,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml>
+</file>
+
+<file path=xl/worksheets/sheet11.xml>
+</file>
+
+<file path=xl/worksheets/sheet12.xml>
+</file>
+
+<file path=xl/worksheets/sheet13.xml>
+</file>
+
+<file path=xl/worksheets/sheet14.xml>
+</file>
+
+<file path=xl/worksheets/sheet15.xml>
+</file>
+
+<file path=xl/worksheets/sheet16.xml>
+</file>
+
+<file path=xl/worksheets/sheet2.xml>
+</file>
+
+<file path=xl/worksheets/sheet3.xml>
+</file>
+
+<file path=xl/worksheets/sheet4.xml>
+</file>
+
+<file path=xl/worksheets/sheet5.xml>
+</file>
+
+<file path=xl/worksheets/sheet6.xml>
+</file>
+
+<file path=xl/worksheets/sheet7.xml>
+</file>
+
+<file path=xl/worksheets/sheet8.xml>
+</file>
+
+<file path=xl/worksheets/sheet9.xml>
 </file>
</xml_diff>